<commit_message>
finishing fixing for daily silo row materials
</commit_message>
<xml_diff>
--- a/apps/analysis/formats/format_QC_SPC_v2.xlsx
+++ b/apps/analysis/formats/format_QC_SPC_v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programing\a1leader\y_data_assistant\analysis\formats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programing\python\a1leader\y_data_assistant\apps\analysis\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569AE559-71B3-479E-BBA3-6D2C2D8B188E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85A78A1-9868-49F4-B495-F48CFEF36B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1816,6 +1816,69 @@
     <xf numFmtId="10" fontId="30" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="30" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="30" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -1827,69 +1890,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="30" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="30" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1899,7 +1899,21 @@
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2029,20 +2043,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -2051,34 +2051,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6454,14 +6426,14 @@
       <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="118" t="s">
+      <c r="B2" s="125"/>
+      <c r="C2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="120"/>
+      <c r="D2" s="109"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -6478,60 +6450,60 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="123"/>
-      <c r="B4" s="126"/>
+      <c r="A4" s="112"/>
+      <c r="B4" s="115"/>
       <c r="C4" s="26"/>
       <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="124"/>
-      <c r="B5" s="127"/>
+      <c r="A5" s="113"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="26"/>
       <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="124"/>
-      <c r="B6" s="127"/>
+      <c r="A6" s="113"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="26"/>
       <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="124"/>
-      <c r="B7" s="127"/>
+      <c r="A7" s="113"/>
+      <c r="B7" s="116"/>
       <c r="C7" s="26"/>
       <c r="D7" s="19"/>
     </row>
     <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="124"/>
-      <c r="B8" s="127"/>
+      <c r="A8" s="113"/>
+      <c r="B8" s="116"/>
       <c r="C8" s="26"/>
       <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="124"/>
-      <c r="B9" s="127"/>
+      <c r="A9" s="113"/>
+      <c r="B9" s="116"/>
       <c r="C9" s="26"/>
       <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="124"/>
-      <c r="B10" s="127"/>
+      <c r="A10" s="113"/>
+      <c r="B10" s="116"/>
       <c r="C10" s="26"/>
       <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="125"/>
-      <c r="B11" s="128"/>
+      <c r="A11" s="114"/>
+      <c r="B11" s="117"/>
       <c r="C11" s="27"/>
       <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="118" t="s">
+      <c r="A12" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="119"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="120"/>
+      <c r="B12" s="126"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="109"/>
     </row>
     <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
@@ -6548,50 +6520,50 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="110"/>
-      <c r="B14" s="113"/>
+      <c r="A14" s="118"/>
+      <c r="B14" s="121"/>
       <c r="C14" s="26"/>
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="111"/>
-      <c r="B15" s="114"/>
+      <c r="A15" s="119"/>
+      <c r="B15" s="122"/>
       <c r="C15" s="26"/>
       <c r="D15" s="19"/>
     </row>
     <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="111"/>
-      <c r="B16" s="114"/>
+      <c r="A16" s="119"/>
+      <c r="B16" s="122"/>
       <c r="C16" s="26"/>
       <c r="D16" s="19"/>
     </row>
     <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="111"/>
-      <c r="B17" s="114"/>
+      <c r="A17" s="119"/>
+      <c r="B17" s="122"/>
       <c r="C17" s="26"/>
       <c r="D17" s="19"/>
     </row>
     <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="111"/>
-      <c r="B18" s="114"/>
+      <c r="A18" s="119"/>
+      <c r="B18" s="122"/>
       <c r="C18" s="26"/>
       <c r="D18" s="19"/>
     </row>
     <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="111"/>
-      <c r="B19" s="114"/>
+      <c r="A19" s="119"/>
+      <c r="B19" s="122"/>
       <c r="C19" s="26"/>
       <c r="D19" s="19"/>
     </row>
     <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="111"/>
-      <c r="B20" s="114"/>
+      <c r="A20" s="119"/>
+      <c r="B20" s="122"/>
       <c r="C20" s="26"/>
       <c r="D20" s="19"/>
     </row>
     <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="112"/>
-      <c r="B21" s="115"/>
+      <c r="A21" s="120"/>
+      <c r="B21" s="123"/>
       <c r="C21" s="26"/>
       <c r="D21" s="19"/>
     </row>
@@ -6600,12 +6572,12 @@
       <c r="D22" s="29"/>
     </row>
     <row r="23" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="118" t="s">
+      <c r="A23" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="120"/>
-      <c r="C23" s="121"/>
-      <c r="D23" s="122"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="110"/>
+      <c r="D23" s="111"/>
     </row>
     <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
@@ -6622,50 +6594,50 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A25" s="110"/>
-      <c r="B25" s="113"/>
+      <c r="A25" s="118"/>
+      <c r="B25" s="121"/>
       <c r="C25" s="26"/>
       <c r="D25" s="19"/>
     </row>
     <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="111"/>
-      <c r="B26" s="114"/>
+      <c r="A26" s="119"/>
+      <c r="B26" s="122"/>
       <c r="C26" s="26"/>
       <c r="D26" s="19"/>
     </row>
     <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="111"/>
-      <c r="B27" s="114"/>
+      <c r="A27" s="119"/>
+      <c r="B27" s="122"/>
       <c r="C27" s="26"/>
       <c r="D27" s="19"/>
     </row>
     <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="111"/>
-      <c r="B28" s="114"/>
+      <c r="A28" s="119"/>
+      <c r="B28" s="122"/>
       <c r="C28" s="26"/>
       <c r="D28" s="19"/>
     </row>
     <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A29" s="111"/>
-      <c r="B29" s="114"/>
+      <c r="A29" s="119"/>
+      <c r="B29" s="122"/>
       <c r="C29" s="26"/>
       <c r="D29" s="19"/>
     </row>
     <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="111"/>
-      <c r="B30" s="114"/>
+      <c r="A30" s="119"/>
+      <c r="B30" s="122"/>
       <c r="C30" s="26"/>
       <c r="D30" s="19"/>
     </row>
     <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A31" s="111"/>
-      <c r="B31" s="114"/>
+      <c r="A31" s="119"/>
+      <c r="B31" s="122"/>
       <c r="C31" s="26"/>
       <c r="D31" s="19"/>
     </row>
     <row r="32" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="112"/>
-      <c r="B32" s="115"/>
+      <c r="A32" s="120"/>
+      <c r="B32" s="123"/>
       <c r="C32" s="27"/>
       <c r="D32" s="20"/>
     </row>
@@ -6682,79 +6654,67 @@
         <v>7</v>
       </c>
       <c r="B34" s="15"/>
-      <c r="C34" s="106"/>
-      <c r="D34" s="107"/>
+      <c r="C34" s="127"/>
+      <c r="D34" s="128"/>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="13"/>
-      <c r="C35" s="106"/>
-      <c r="D35" s="107"/>
+      <c r="C35" s="127"/>
+      <c r="D35" s="128"/>
     </row>
     <row r="36" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B36" s="10"/>
-      <c r="C36" s="106"/>
-      <c r="D36" s="107"/>
+      <c r="C36" s="127"/>
+      <c r="D36" s="128"/>
     </row>
     <row r="37" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B37" s="8"/>
-      <c r="C37" s="106"/>
-      <c r="D37" s="107"/>
+      <c r="C37" s="127"/>
+      <c r="D37" s="128"/>
     </row>
     <row r="38" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B38" s="9"/>
-      <c r="C38" s="106"/>
-      <c r="D38" s="107"/>
+      <c r="C38" s="127"/>
+      <c r="D38" s="128"/>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B39" s="11"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="107"/>
+      <c r="C39" s="127"/>
+      <c r="D39" s="128"/>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B40" s="12"/>
-      <c r="C40" s="106"/>
-      <c r="D40" s="107"/>
+      <c r="C40" s="127"/>
+      <c r="D40" s="128"/>
     </row>
     <row r="41" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B41" s="14"/>
-      <c r="C41" s="108"/>
-      <c r="D41" s="109"/>
+      <c r="C41" s="129"/>
+      <c r="D41" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="A14:A21"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="B25:B32"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A23:B23"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
@@ -6763,6 +6723,18 @@
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="B14:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6895,11 +6867,11 @@
       <c r="C18" s="94"/>
       <c r="D18" s="95"/>
       <c r="E18" s="95"/>
-      <c r="F18" s="129"/>
+      <c r="F18" s="106"/>
       <c r="H18" s="80"/>
       <c r="I18" s="80"/>
       <c r="J18" s="80"/>
-      <c r="K18" s="130"/>
+      <c r="K18" s="107"/>
       <c r="M18" s="104"/>
       <c r="N18" s="82"/>
       <c r="O18" s="83"/>
@@ -6912,11 +6884,11 @@
       <c r="C19" s="94"/>
       <c r="D19" s="95"/>
       <c r="E19" s="95"/>
-      <c r="F19" s="129"/>
+      <c r="F19" s="106"/>
       <c r="H19" s="80"/>
       <c r="I19" s="80"/>
       <c r="J19" s="80"/>
-      <c r="K19" s="130"/>
+      <c r="K19" s="107"/>
       <c r="M19" s="104"/>
       <c r="N19" s="82"/>
       <c r="O19" s="83"/>
@@ -6929,11 +6901,11 @@
       <c r="C20" s="94"/>
       <c r="D20" s="95"/>
       <c r="E20" s="95"/>
-      <c r="F20" s="129"/>
+      <c r="F20" s="106"/>
       <c r="H20" s="80"/>
       <c r="I20" s="80"/>
       <c r="J20" s="80"/>
-      <c r="K20" s="130"/>
+      <c r="K20" s="107"/>
       <c r="M20" s="104"/>
       <c r="N20" s="82"/>
       <c r="O20" s="83"/>
@@ -6946,11 +6918,11 @@
       <c r="C21" s="94"/>
       <c r="D21" s="95"/>
       <c r="E21" s="95"/>
-      <c r="F21" s="129"/>
+      <c r="F21" s="106"/>
       <c r="H21" s="80"/>
       <c r="I21" s="80"/>
       <c r="J21" s="80"/>
-      <c r="K21" s="130"/>
+      <c r="K21" s="107"/>
       <c r="M21" s="104"/>
       <c r="N21" s="82"/>
       <c r="O21" s="83"/>
@@ -6963,11 +6935,11 @@
       <c r="C22" s="94"/>
       <c r="D22" s="95"/>
       <c r="E22" s="95"/>
-      <c r="F22" s="129"/>
+      <c r="F22" s="106"/>
       <c r="H22" s="80"/>
       <c r="I22" s="80"/>
       <c r="J22" s="80"/>
-      <c r="K22" s="130"/>
+      <c r="K22" s="107"/>
       <c r="M22" s="104"/>
       <c r="N22" s="82"/>
       <c r="O22" s="83"/>
@@ -6980,11 +6952,11 @@
       <c r="C23" s="94"/>
       <c r="D23" s="95"/>
       <c r="E23" s="95"/>
-      <c r="F23" s="129"/>
+      <c r="F23" s="106"/>
       <c r="H23" s="80"/>
       <c r="I23" s="80"/>
       <c r="J23" s="80"/>
-      <c r="K23" s="130"/>
+      <c r="K23" s="107"/>
       <c r="M23" s="104"/>
       <c r="N23" s="82"/>
       <c r="O23" s="83"/>
@@ -6997,11 +6969,11 @@
       <c r="C24" s="94"/>
       <c r="D24" s="95"/>
       <c r="E24" s="95"/>
-      <c r="F24" s="129"/>
+      <c r="F24" s="106"/>
       <c r="H24" s="80"/>
       <c r="I24" s="80"/>
       <c r="J24" s="80"/>
-      <c r="K24" s="130"/>
+      <c r="K24" s="107"/>
       <c r="M24" s="104"/>
       <c r="N24" s="82"/>
       <c r="O24" s="83"/>
@@ -7014,11 +6986,11 @@
       <c r="C25" s="94"/>
       <c r="D25" s="95"/>
       <c r="E25" s="95"/>
-      <c r="F25" s="129"/>
+      <c r="F25" s="106"/>
       <c r="H25" s="80"/>
       <c r="I25" s="80"/>
       <c r="J25" s="80"/>
-      <c r="K25" s="130"/>
+      <c r="K25" s="107"/>
       <c r="M25" s="104"/>
       <c r="N25" s="82"/>
       <c r="O25" s="83"/>
@@ -7031,11 +7003,11 @@
       <c r="C26" s="94"/>
       <c r="D26" s="95"/>
       <c r="E26" s="95"/>
-      <c r="F26" s="129"/>
+      <c r="F26" s="106"/>
       <c r="H26" s="80"/>
       <c r="I26" s="80"/>
       <c r="J26" s="80"/>
-      <c r="K26" s="130"/>
+      <c r="K26" s="107"/>
       <c r="M26" s="104"/>
       <c r="N26" s="82"/>
       <c r="O26" s="83"/>
@@ -7048,11 +7020,11 @@
       <c r="C27" s="94"/>
       <c r="D27" s="95"/>
       <c r="E27" s="95"/>
-      <c r="F27" s="129"/>
+      <c r="F27" s="106"/>
       <c r="H27" s="80"/>
       <c r="I27" s="80"/>
       <c r="J27" s="80"/>
-      <c r="K27" s="130"/>
+      <c r="K27" s="107"/>
       <c r="M27" s="104"/>
       <c r="N27" s="82"/>
       <c r="O27" s="83"/>
@@ -7065,11 +7037,11 @@
       <c r="C28" s="94"/>
       <c r="D28" s="95"/>
       <c r="E28" s="95"/>
-      <c r="F28" s="129"/>
+      <c r="F28" s="106"/>
       <c r="H28" s="80"/>
       <c r="I28" s="80"/>
       <c r="J28" s="80"/>
-      <c r="K28" s="130"/>
+      <c r="K28" s="107"/>
       <c r="M28" s="104"/>
       <c r="N28" s="82"/>
       <c r="O28" s="83"/>
@@ -7082,11 +7054,11 @@
       <c r="C29" s="94"/>
       <c r="D29" s="95"/>
       <c r="E29" s="95"/>
-      <c r="F29" s="129"/>
+      <c r="F29" s="106"/>
       <c r="H29" s="80"/>
       <c r="I29" s="80"/>
       <c r="J29" s="80"/>
-      <c r="K29" s="130"/>
+      <c r="K29" s="107"/>
       <c r="M29" s="104"/>
       <c r="N29" s="82"/>
       <c r="O29" s="83"/>
@@ -7099,11 +7071,11 @@
       <c r="C30" s="94"/>
       <c r="D30" s="95"/>
       <c r="E30" s="95"/>
-      <c r="F30" s="129"/>
+      <c r="F30" s="106"/>
       <c r="H30" s="80"/>
       <c r="I30" s="80"/>
       <c r="J30" s="80"/>
-      <c r="K30" s="130"/>
+      <c r="K30" s="107"/>
       <c r="M30" s="104"/>
       <c r="N30" s="82"/>
       <c r="O30" s="83"/>
@@ -7116,11 +7088,11 @@
       <c r="C31" s="94"/>
       <c r="D31" s="95"/>
       <c r="E31" s="95"/>
-      <c r="F31" s="129"/>
+      <c r="F31" s="106"/>
       <c r="H31" s="80"/>
       <c r="I31" s="80"/>
       <c r="J31" s="80"/>
-      <c r="K31" s="130"/>
+      <c r="K31" s="107"/>
       <c r="M31" s="104"/>
       <c r="N31" s="82"/>
       <c r="O31" s="83"/>
@@ -7133,11 +7105,11 @@
       <c r="C32" s="94"/>
       <c r="D32" s="95"/>
       <c r="E32" s="95"/>
-      <c r="F32" s="129"/>
+      <c r="F32" s="106"/>
       <c r="H32" s="80"/>
       <c r="I32" s="80"/>
       <c r="J32" s="80"/>
-      <c r="K32" s="130"/>
+      <c r="K32" s="107"/>
       <c r="M32" s="104"/>
       <c r="N32" s="82"/>
       <c r="O32" s="83"/>
@@ -7150,11 +7122,11 @@
       <c r="C33" s="94"/>
       <c r="D33" s="95"/>
       <c r="E33" s="95"/>
-      <c r="F33" s="129"/>
+      <c r="F33" s="106"/>
       <c r="H33" s="80"/>
       <c r="I33" s="80"/>
       <c r="J33" s="80"/>
-      <c r="K33" s="130"/>
+      <c r="K33" s="107"/>
       <c r="M33" s="104"/>
       <c r="N33" s="82"/>
       <c r="O33" s="83"/>
@@ -7167,11 +7139,11 @@
       <c r="C34" s="94"/>
       <c r="D34" s="95"/>
       <c r="E34" s="95"/>
-      <c r="F34" s="129"/>
+      <c r="F34" s="106"/>
       <c r="H34" s="80"/>
       <c r="I34" s="80"/>
       <c r="J34" s="80"/>
-      <c r="K34" s="130"/>
+      <c r="K34" s="107"/>
       <c r="M34" s="104"/>
       <c r="N34" s="82"/>
       <c r="O34" s="83"/>
@@ -7184,11 +7156,11 @@
       <c r="C35" s="94"/>
       <c r="D35" s="95"/>
       <c r="E35" s="95"/>
-      <c r="F35" s="129"/>
+      <c r="F35" s="106"/>
       <c r="H35" s="80"/>
       <c r="I35" s="80"/>
       <c r="J35" s="80"/>
-      <c r="K35" s="130"/>
+      <c r="K35" s="107"/>
       <c r="M35" s="104"/>
       <c r="N35" s="82"/>
       <c r="O35" s="83"/>
@@ -7201,11 +7173,11 @@
       <c r="C36" s="94"/>
       <c r="D36" s="95"/>
       <c r="E36" s="95"/>
-      <c r="F36" s="129"/>
+      <c r="F36" s="106"/>
       <c r="H36" s="80"/>
       <c r="I36" s="80"/>
       <c r="J36" s="80"/>
-      <c r="K36" s="130"/>
+      <c r="K36" s="107"/>
       <c r="M36" s="104"/>
       <c r="N36" s="82"/>
       <c r="O36" s="83"/>
@@ -7218,11 +7190,11 @@
       <c r="C37" s="94"/>
       <c r="D37" s="95"/>
       <c r="E37" s="95"/>
-      <c r="F37" s="129"/>
+      <c r="F37" s="106"/>
       <c r="H37" s="80"/>
       <c r="I37" s="80"/>
       <c r="J37" s="80"/>
-      <c r="K37" s="130"/>
+      <c r="K37" s="107"/>
       <c r="M37" s="104"/>
       <c r="N37" s="82"/>
       <c r="O37" s="83"/>
@@ -7235,11 +7207,11 @@
       <c r="C38" s="94"/>
       <c r="D38" s="95"/>
       <c r="E38" s="95"/>
-      <c r="F38" s="129"/>
+      <c r="F38" s="106"/>
       <c r="H38" s="80"/>
       <c r="I38" s="80"/>
       <c r="J38" s="80"/>
-      <c r="K38" s="130"/>
+      <c r="K38" s="107"/>
       <c r="M38" s="104"/>
       <c r="N38" s="82"/>
       <c r="O38" s="83"/>
@@ -7252,11 +7224,11 @@
       <c r="C39" s="94"/>
       <c r="D39" s="95"/>
       <c r="E39" s="95"/>
-      <c r="F39" s="129"/>
+      <c r="F39" s="106"/>
       <c r="H39" s="80"/>
       <c r="I39" s="80"/>
       <c r="J39" s="80"/>
-      <c r="K39" s="130"/>
+      <c r="K39" s="107"/>
       <c r="M39" s="104"/>
       <c r="N39" s="82"/>
       <c r="O39" s="83"/>
@@ -7269,11 +7241,11 @@
       <c r="C40" s="94"/>
       <c r="D40" s="95"/>
       <c r="E40" s="95"/>
-      <c r="F40" s="129"/>
+      <c r="F40" s="106"/>
       <c r="H40" s="80"/>
       <c r="I40" s="80"/>
       <c r="J40" s="80"/>
-      <c r="K40" s="130"/>
+      <c r="K40" s="107"/>
       <c r="M40" s="104"/>
       <c r="N40" s="82"/>
       <c r="O40" s="83"/>
@@ -7378,10 +7350,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:F45">
-    <cfRule type="expression" dxfId="17" priority="19">
+    <cfRule type="expression" dxfId="19" priority="19">
       <formula>#REF!=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
       <formula>#REF!=1</formula>
     </cfRule>
     <cfRule type="expression" priority="22">
@@ -7392,10 +7364,10 @@
     <cfRule type="expression" priority="21">
       <formula>K41=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="23">
+    <cfRule type="expression" dxfId="17" priority="23">
       <formula>#REF!=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="24" stopIfTrue="1">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7403,31 +7375,31 @@
     <cfRule type="expression" priority="15" stopIfTrue="1">
       <formula>F18=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="16" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="16" stopIfTrue="1" operator="lessThan">
       <formula>D18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="17" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="17" stopIfTrue="1" operator="between">
       <formula>D18</formula>
       <formula>E18</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="18" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="18" stopIfTrue="1" operator="greaterThan">
       <formula>E18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="10" stopIfTrue="1">
       <formula>K18&lt;H18</formula>
     </cfRule>
     <cfRule type="expression" priority="11" stopIfTrue="1">
       <formula>K18=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
       <formula>XEZ18=H18</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="13" stopIfTrue="1">
       <formula>K18&gt;H18*1.05</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="14" stopIfTrue="1">
       <formula>K18&lt;H18</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7435,31 +7407,31 @@
     <cfRule type="expression" priority="6" stopIfTrue="1">
       <formula>F19=""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>D19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="between">
       <formula>D19</formula>
       <formula>E19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" stopIfTrue="1" operator="greaterThan">
       <formula>E19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:K40">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>K19&lt;H19</formula>
     </cfRule>
     <cfRule type="expression" priority="2" stopIfTrue="1">
       <formula>K19=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>XEZ19=H19</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>K19&gt;H19*1.05</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
       <formula>K19&lt;H19</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7958,10 +7930,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3:K21">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>C3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>C3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>